<commit_message>
add text in file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="8">
   <si>
     <t xml:space="preserve">@test</t>
   </si>
@@ -159,10 +159,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C92" activeCellId="0" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -231,16 +231,427 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>